<commit_message>
Signed-off-by: Linh Vu <Linh Vu>
</commit_message>
<xml_diff>
--- a/Project/ProjectCheckOfSheet.xlsx
+++ b/Project/ProjectCheckOfSheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KHANH VU\Desktop\GITHUB_CIS5\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,16 +208,37 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -225,32 +246,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,50 +573,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="8.7109375" style="6" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="7"/>
+    <col min="4" max="4" width="30.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="2:7" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="2:7" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -582,355 +630,541 @@
       <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
       <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10" s="4">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11" s="4">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13" s="4">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14" s="4">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15" s="4">
         <v>14</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16" s="4">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17" s="4">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18" s="4">
         <v>17</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>3</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21" s="4">
         <v>2</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22" s="4">
         <v>3</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24" s="4">
         <v>5</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25" s="4">
         <v>6</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26" s="4">
         <v>7</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27" s="4">
         <v>8</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28" s="4">
         <v>9</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29" s="4">
         <v>10</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>4</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32" s="4">
         <v>2</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
       <c r="C33" s="4">
         <v>4</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
       <c r="C34" s="4">
         <v>5</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
       <c r="C35" s="4">
         <v>6</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
       <c r="C36" s="4">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
       <c r="C37" s="4">
         <v>8</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
       <c r="C38" s="4">
         <v>11</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
       <c r="C39" s="4">
         <v>13</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
       <c r="C40" s="4">
         <v>14</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>5</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
       <c r="C43" s="4">
         <v>2</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
       <c r="C44" s="4">
         <v>5</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
       <c r="C45" s="4">
         <v>6</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
       <c r="C46" s="4">
         <v>11</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
       <c r="C47" s="4">
         <v>12</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="80" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>